<commit_message>
actualización de eCommerce y mejoras en carrito
</commit_message>
<xml_diff>
--- a/Assets/sheets/products.xlsx
+++ b/Assets/sheets/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Datos\Curso FE JS 24\.Proyecto Integrador\Assets\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3A9002-261C-4D1B-A814-FC8858033EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39B4B67-3CB2-4BAB-86B4-0749DDBDEF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,30 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
   <si>
     <t>NOMBRE
 (todo en mayúsculas)</t>
   </si>
   <si>
-    <t>PRECIO FINAL SIN IVA
-(En formato $X.XXX)</t>
-  </si>
-  <si>
-    <t>TIENE DESCUENTO? 
-(Valor en X%)</t>
-  </si>
-  <si>
     <t>DESCRIPCION
 BREVE DE PRODUCTO</t>
   </si>
   <si>
     <t>CANTIDAD 
 EN INVENTARIO</t>
-  </si>
-  <si>
-    <t>DESCRIPCION DETALLADA
-DE PRODUCTO</t>
   </si>
   <si>
     <t>../assets/images/Products/</t>
@@ -62,13 +50,120 @@
     <t>IMAGENES PARA CARROUSSEL POPUP
 Especificar ruta relativa de imágenes
  ../assets/images/Products/nombredelaimagen.formato</t>
+  </si>
+  <si>
+    <t>GALLETAS DE AVENA PARA CABALLOS</t>
+  </si>
+  <si>
+    <t>Con un sabor que está justo entre ‘no es pasto’ y ‘esto no huele tan mal’</t>
+  </si>
+  <si>
+    <t>Este es un producto de alta calidad con características avanzadas para premiar a tu corcel por hacerte ganar 5 likes en tiktok.</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>ARMADURA DORADA PARA CABALLOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin dudas la peor decision de la humanidad desde el rechazo de Blockbuster a Netflix.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Porque a nadie con dos dedos de frente se le ocurriria capitalizar hobbies.
+</t>
+  </si>
+  <si>
+    <t>../assets/images/Products/horsearmor.webp</t>
+  </si>
+  <si>
+    <t>$15.500,00</t>
+  </si>
+  <si>
+    <t>../assets/images/Products/cookies.png</t>
+  </si>
+  <si>
+    <t>SHAMPOO EQUINO</t>
+  </si>
+  <si>
+    <t>Porque si alguien aquí merece una melena de ensueño, es definitivamente él, no tú.</t>
+  </si>
+  <si>
+    <t>Con este shampoo, su melena será la envidia del establo mientras tú sigues lidiando con el frizz en silencio. ¡El lujo que tú no puedes darte, pero él sí!</t>
+  </si>
+  <si>
+    <t>../assets/images/Products/noimgprod.webp</t>
+  </si>
+  <si>
+    <t>$32.000,00</t>
+  </si>
+  <si>
+    <t>$180.600,00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIENE DESCUENTO? 
+(Valor en X% 
+Dejar Vacio si no posee descuento)
+</t>
+  </si>
+  <si>
+    <t>MONTURA PARA CERDOS</t>
+  </si>
+  <si>
+    <t>resistente y adecuada para recorridos cortos. No esperes velocidad ni comodidad extra; cumple su función y punto.</t>
+  </si>
+  <si>
+    <t>DESCRIPCION DETALLADA
+DE PRODUCTO
+(Dejar vacio si no hay detalles adicionales)</t>
+  </si>
+  <si>
+    <t>../assets/images/Products/saddlecraft.webp</t>
+  </si>
+  <si>
+    <t>FR-33 0FL1C3</t>
+  </si>
+  <si>
+    <t>Sin Pulgas, Sin Corazón, Sin Problemas.</t>
+  </si>
+  <si>
+    <t>../assets/images/Products/robodog.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalmente, un perro que no ladra, no muerde y jamás te juzga... aunque tampoco te quiere. Este robot perro sigue órdenes, no se roba tu cama y, lo mejor de todo, no necesita visitas al veterinario. Perfecto para quienes aman la idea de un perro, pero no el compromiso.
+</t>
+  </si>
+  <si>
+    <t>$28.600,00</t>
+  </si>
+  <si>
+    <t>CREMA PARA PELO EQUINO</t>
+  </si>
+  <si>
+    <t>Dale a tu caballo ese brillo que tú solo sueñas tener con nuestra crema.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Porque si alguien aquí merece una melena de ensueño, es definitivamente él, no tú. ¡Y con un aroma que hará que los demás en el establo lo envidien!
+</t>
+  </si>
+  <si>
+    <t>PRECIO FINAL SIN IVA 21%
+(En formato $X.XXX,XX)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORREA </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +178,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="4">
@@ -117,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -130,6 +230,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -411,153 +529,380 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="61.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="35" style="1" customWidth="1"/>
-    <col min="8" max="8" width="39.42578125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="60.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="61.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="46.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="61.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="35" style="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1">
+        <v>50</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1">
+        <v>10</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1">
+        <v>132</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="1">
+        <v>150</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1">
+        <v>10</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="1">
+        <v>120</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="1">
+        <v>120</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>6</v>
+      <c r="D9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>